<commit_message>
okay so maybe i was the problem
</commit_message>
<xml_diff>
--- a/Resources/regression results.xlsx
+++ b/Resources/regression results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e7cb72b1a048b4d/Desktop/Data Science Bootcamp/Projects/Project 4/Project_4-Group_1/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{22D2C061-AD3A-4F00-B43A-18532FDDB02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE58757B-FECF-47AF-8536-FE4C2B0DD384}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{22D2C061-AD3A-4F00-B43A-18532FDDB02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A538740-6837-4080-B3A5-9AA1BA1BF448}"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="1290" windowWidth="21615" windowHeight="18330" activeTab="3" xr2:uid="{58A401A9-D6E0-4094-8908-79C7B918D204}"/>
+    <workbookView xWindow="4890" yWindow="1680" windowWidth="21615" windowHeight="18330" activeTab="3" xr2:uid="{58A401A9-D6E0-4094-8908-79C7B918D204}"/>
   </bookViews>
   <sheets>
     <sheet name="Training | Testing" sheetId="1" r:id="rId1"/>
@@ -3594,8 +3594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0849AC72-80B0-4C84-A9B7-1CAE8A9C27CA}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:E45"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4708,7 +4708,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4783,16 +4783,16 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.99765359674999998</v>
+        <v>0.68436135374999996</v>
       </c>
       <c r="C5">
-        <v>0.70350642050000001</v>
+        <v>0.68436135374999996</v>
       </c>
       <c r="D5">
-        <v>0.99968168449999995</v>
+        <v>0.84083503724999997</v>
       </c>
       <c r="E5">
-        <v>0.85582798650000003</v>
+        <v>0.84083503724999997</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>